<commit_message>
P6 Update notes file
</commit_message>
<xml_diff>
--- a/Euler Project Answers/Project Euler - Problem 6 - Notes.xlsx
+++ b/Euler Project Answers/Project Euler - Problem 6 - Notes.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Foundation Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Sum squared = cubes sumed" sheetId="3" r:id="rId2"/>
+    <sheet name="Squares as Function of Prior" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="160">
   <si>
     <t>Number</t>
   </si>
@@ -668,13 +669,2296 @@
       </rPr>
       <t xml:space="preserve">(n-0) </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-2) - 1 + 2n + 2(-1) - 1 + 2n - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-2) - 1 + 2n + 2(-1) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-2) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) + 2(-2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n) + 2(-1) + 2(-2) + 2(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-3) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-3) - 1 + 2n + 2(-2) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 + 2n + 2(-1) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 + 2n + 2(-1) - 1 + 2n - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) + 2(-3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n) + 2(-1) + 2(-3) + 2(-2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n) + 3(-1) + 2(-3) + 2(-2) + 2(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-4) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 + 2n + 2(-1) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 + 2n + 2(-1) - 1 + 2n - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) + 2(-4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n) + 2(-1) + 2(-4) + 2(-3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n) + 3(-1) + 2(-4) + 2(-3) + 2(-2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n) + 4(-1) + 2(-4) + 2(-3) + 2(-2) + 2(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 + 2n + 2(-4) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 + 2n + 2(-4) - 1 + 2n + 2(-3) - 1  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 + 2n + 2(-2) - 1 + 2n + 2(-1) - 1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-5) - 1 + 2n + 2(-4) - 1 + 2n + 2(-3) - 1 +  2n + 2(-2) - 1 + 2n + 2(-1) - 1 + 2n - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) + 2(-5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n) + 2(-1) + 2(-5) + 2(-4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n) + 3(-1) + 2(-5) + 2(-4) + 2(-3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n) + 4(-1) + 2(-5) + 2(-4) + 2(-3) + 2(-2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 5(2n) + 5(-1) + 2(-5) + 2(-4) + 2(-3) + 2(-2) + 2(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(n-2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(n-3) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92CDDC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n) + 0(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n) + 3(-1) + 2(-2) + 2(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n) + 4(-1) + 2(-3) + 2(-2) + 2(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 5(2n) + 5(-1) + 2(-4) + 2(-3) + 2(-2) + 2(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 6(2n) + 6(-1) + 2(-5) + 2(-4) + 2(-3) + 2(-2) + 2(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) + -2(3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n - 1) + -2(3 + 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n - 1) + -2(3 + 2 + 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-4)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n - 1) + -2(3 + 2 + 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-(n-start))</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + (2n - 1)(sum(0, n-1)) + -2(figure this </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) + -2(2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n - 1) + -2(2 + 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n - 1) + -2(2 + 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) + -2(4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n - 1) + -2(4 + 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n - 1) + -2(4 + 3 + 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n - 1) + -2(4 + 3 + 2 + 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 5(2n - 1) + -2(4 + 3 + 2 + 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-5)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF92CDDC"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) + -2(5)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n - 1) + -2(5 + 4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 3(2n - 1) + -2(5 + 4 + 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 4(2n - 1) + -2(5 + 4 + 3 + 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 5(2n - 1) + -2(5 + 4 + 3 + 2 + 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-6)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 6(2n - 1) + -2(5 + 4 + 3 + 2 + 1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(n-2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-1) - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2n + 2(-1) - 1 + 2n - 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n) + 2(-1) + 2(-1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 2(-0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n) + 1(-1) + 2(-1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) + -2(1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2(2n - 1) + -2(1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(n-3) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ 0(2n - 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(n-1)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 1(2n - 1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ -2(0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>x = n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>(last part needs to be an equation, not iteration, otherwise just run initial iteration)</t>
+  </si>
+  <si>
+    <t>Sum Square</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>(1+2+3+4+…)^2</t>
+  </si>
+  <si>
+    <t>(1)^2</t>
+  </si>
+  <si>
+    <t>1^2</t>
+  </si>
+  <si>
+    <t>1^3 + 2^3 + 3^3 + 4^3 + …</t>
+  </si>
+  <si>
+    <t>1^3</t>
+  </si>
+  <si>
+    <t>(1+2)^2</t>
+  </si>
+  <si>
+    <t>3^2</t>
+  </si>
+  <si>
+    <t>2^3</t>
+  </si>
+  <si>
+    <t>(1+2+3)^2</t>
+  </si>
+  <si>
+    <t>(1+2+3+4)^2</t>
+  </si>
+  <si>
+    <t>(1+2+3+4+5)^2</t>
+  </si>
+  <si>
+    <t>(1+2+3+4+5+6)^2</t>
+  </si>
+  <si>
+    <t>6^2</t>
+  </si>
+  <si>
+    <t>10^2</t>
+  </si>
+  <si>
+    <t>15^2</t>
+  </si>
+  <si>
+    <t>21^2</t>
+  </si>
+  <si>
+    <t>3^3</t>
+  </si>
+  <si>
+    <t>4^3</t>
+  </si>
+  <si>
+    <t>5^3</t>
+  </si>
+  <si>
+    <t>6^3</t>
+  </si>
+  <si>
+    <t>(1+2)(1+2)</t>
+  </si>
+  <si>
+    <t>1(1) + 1(2) + 1(2) + 2(2)</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>When multiplying, write the smaller number as the coefficient, and write squares as x(x).</t>
+  </si>
+  <si>
+    <t>1(1) + 4(2)</t>
+  </si>
+  <si>
+    <t>1 + 2(2)(2)</t>
+  </si>
+  <si>
+    <t>1^x + 2^3</t>
+  </si>
+  <si>
+    <t>(1+2+3)(1+2+3)</t>
+  </si>
+  <si>
+    <t>1(1) + 1(2) + 1(3) + 1(2) + 2(2) + 2(3) + 1(3) + 2(3) + 3(3)</t>
+  </si>
+  <si>
+    <t>1(1) + 1(2) + 1(2) + 2(2) + 1(3) + 2(3) + 1(3) + 2(3) + 3(3)</t>
+  </si>
+  <si>
+    <t>1(1) + 4(2) + 9(3)</t>
+  </si>
+  <si>
+    <t>1 + 2(2)(2) + (3)(3)(3)</t>
+  </si>
+  <si>
+    <t>1^x + 2^3 + 3^3</t>
+  </si>
+  <si>
+    <t>(1+2+3+4)(1+2+3+4)</t>
+  </si>
+  <si>
+    <t>1(1) + 1(2) + 1(3) + 1(4) + 1(2) + 2(2) + 2(3) + 2(4) + 1(3) + 2(3) + 3(3) + 3(4) + 1(4) + 2(4) + 3(4) + 4(4)</t>
+  </si>
+  <si>
+    <t>1(1) + 1(2) + 1(2) + 2(2) + 1(3) + 2(3) + 1(3) + 2(3) + 3(3) + 1(4) + 2(4) + 3(4) + 1(4) + 2(4) + 3(4) + 4(4)</t>
+  </si>
+  <si>
+    <t>1(1) + 4(2) + 9(3) + 16(4)</t>
+  </si>
+  <si>
+    <t>1 + 2(2)(2) + 3(3)(3) + 4(4)(4)</t>
+  </si>
+  <si>
+    <t>1^x + 2^3 + 3^3 + 4^3</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Because (1+2+3+…)^2 = (1^3 + 2^3 + 3^3 + …) (see next sheet)</t>
+  </si>
+  <si>
+    <t>(1+2+3…)^2 increases by x^3 each time</t>
+  </si>
+  <si>
+    <t>(1^2 + 2^2 + 3^3 + …) increases by x^2 each time</t>
+  </si>
+  <si>
+    <t>Therefore, difference between (1+2+3+…)^2 and (1^2 + 2^2 + 3^2 + …)</t>
+  </si>
+  <si>
+    <t>increases by x^3 - x^2 each time</t>
+  </si>
+  <si>
+    <t>Thus for any number x</t>
+  </si>
+  <si>
+    <t>difference can be found by iterating (x^3 - x^2) and adding to previous result from 1 to x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -726,13 +3010,64 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92CDDC"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -777,7 +3112,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -877,8 +3212,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -895,11 +3344,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="213">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -949,6 +3406,63 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -998,6 +3512,63 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1327,58 +3898,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <f>B1+C2</f>
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <f t="shared" ref="D1:K1" si="0">C1+D2</f>
-        <v>6</v>
-      </c>
-      <c r="E1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="G1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="H1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="I1">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="J1">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="K1">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
+    <row r="1" spans="1:11" ht="16" thickBot="1"/>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -1414,93 +3942,262 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>B4+C2</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f>C4+D2</f>
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f>D4+E2</f>
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f>E4+F2</f>
+        <v>15</v>
+      </c>
+      <c r="G4">
+        <f>F4+G2</f>
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <f>G4+H2</f>
+        <v>28</v>
+      </c>
+      <c r="I4">
+        <f>H4+I2</f>
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <f>I4+J2</f>
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <f>J4+K2</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5">
+        <f>B4^2</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:K5" si="0">C4^2</f>
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>784</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1296</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>3025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B10">
         <f>B2^2</f>
         <v>1</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:D3" si="1">C2^2</f>
+      <c r="C10">
+        <f>C2^2</f>
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="D10">
+        <f>D2^2</f>
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <f>E2^2</f>
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <f>F2^2</f>
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <f>G2^2</f>
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <f>H2^2</f>
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <f>I2^2</f>
+        <v>64</v>
+      </c>
+      <c r="J10">
+        <f>J2^2</f>
+        <v>81</v>
+      </c>
+      <c r="K10">
+        <f>K2^2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>B11+C10</f>
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:K11" si="1">C11+D10</f>
+        <v>14</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="2">E2^2</f>
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3" si="3">F2^2</f>
-        <v>25</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3" si="4">G2^2</f>
-        <v>36</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3" si="5">H2^2</f>
-        <v>49</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3" si="6">I2^2</f>
-        <v>64</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3" si="7">J2^2</f>
-        <v>81</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3" si="8">K2^2</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f>B4+C3</f>
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:K4" si="9">C4+D3</f>
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="9"/>
+      <c r="F11">
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="9"/>
+      <c r="G11">
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="9"/>
+      <c r="H11">
+        <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="9"/>
+      <c r="I11">
+        <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="9"/>
+      <c r="J11">
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="9"/>
+      <c r="K11">
+        <f t="shared" si="1"/>
         <v>385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16">
+        <f>B5-B11</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:K16" si="2">C5-C11</f>
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>644</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>1092</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>1740</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1516,17 +4213,310 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" s="13" customFormat="1" ht="20">
+      <c r="B2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5">
+        <f>1^2</f>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5">
+        <f>1^3</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>J4+I5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6">
+        <f>3^2</f>
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6">
+        <f>2^3</f>
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J10" si="0">J5+I6</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <f>6^2</f>
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <f>3^3</f>
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8">
+        <f>10^2</f>
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8">
+        <f>4^3</f>
+        <v>64</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9">
+        <f>15^2</f>
+        <v>225</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9">
+        <f>5^3</f>
+        <v>125</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10">
+        <f>21^2</f>
+        <v>441</v>
+      </c>
+      <c r="H10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10">
+        <f>6^3</f>
+        <v>216</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E20" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" t="s">
+        <v>138</v>
+      </c>
+      <c r="E22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
+      <c r="I24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X52"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="23.1640625" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="12" width="22.1640625" customWidth="1"/>
-    <col min="15" max="15" width="32.6640625" customWidth="1"/>
+    <col min="15" max="15" width="35.33203125" customWidth="1"/>
     <col min="18" max="18" width="43.83203125" customWidth="1"/>
     <col min="21" max="21" width="52.83203125" customWidth="1"/>
     <col min="24" max="24" width="63.33203125" customWidth="1"/>
@@ -1699,173 +4689,484 @@
         <v>385</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="3" customFormat="1">
-      <c r="A9" s="8">
+    <row r="7" spans="1:24" ht="17">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="11" customFormat="1">
+      <c r="A10" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="D9" s="8">
+      <c r="B10" s="10"/>
+      <c r="D10" s="10">
         <v>2</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="I9" s="8">
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="I10" s="10">
         <v>3</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="O9" s="8">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="O10" s="10">
         <v>4</v>
       </c>
-      <c r="R9" s="8">
+      <c r="R10" s="10">
         <v>5</v>
       </c>
-      <c r="U9" s="8">
+      <c r="U10" s="10">
         <v>6</v>
       </c>
-      <c r="V9"/>
-      <c r="X9" s="8">
+      <c r="V10" s="12"/>
+      <c r="X10" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:24" s="7" customFormat="1">
-      <c r="B10" s="7">
+    <row r="11" spans="1:24" s="7" customFormat="1">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="7">
         <v>2</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J11" s="7">
         <v>1</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K11" s="7">
         <v>2</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L11" s="7">
         <v>3</v>
       </c>
-      <c r="V10"/>
-    </row>
-    <row r="11" spans="1:24" ht="17">
-      <c r="B11" t="s">
+      <c r="V11"/>
+    </row>
+    <row r="12" spans="1:24" ht="17">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>6</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>8</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>9</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="17">
+    <row r="14" spans="1:24" ht="16">
       <c r="A14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="17">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>8</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O15" t="s">
         <v>10</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R15" t="s">
         <v>18</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U15" t="s">
         <v>20</v>
       </c>
-      <c r="X14" t="s">
+      <c r="X15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="17">
-      <c r="D15" t="s">
+    <row r="16" spans="1:24" ht="17">
+      <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>9</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O16" t="s">
         <v>11</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R16" t="s">
         <v>17</v>
       </c>
-      <c r="U15" t="s">
+      <c r="U16" t="s">
         <v>21</v>
       </c>
-      <c r="X15" t="s">
+      <c r="X16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17">
-      <c r="I16" t="s">
+    <row r="17" spans="1:24" ht="17">
+      <c r="I17" t="s">
         <v>12</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O17" t="s">
         <v>14</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R17" t="s">
         <v>16</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U17" t="s">
         <v>24</v>
       </c>
-      <c r="X16" t="s">
+      <c r="X17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="15:24" ht="17">
-      <c r="O17" t="s">
+    <row r="18" spans="1:24" ht="17">
+      <c r="O18" t="s">
         <v>13</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R18" t="s">
         <v>15</v>
       </c>
-      <c r="U17" t="s">
+      <c r="U18" t="s">
         <v>25</v>
       </c>
-      <c r="X17" t="s">
+      <c r="X18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="15:24" ht="17">
-      <c r="R18" t="s">
+    <row r="19" spans="1:24" ht="17">
+      <c r="R19" t="s">
         <v>19</v>
       </c>
-      <c r="U18" t="s">
+      <c r="U19" t="s">
         <v>22</v>
       </c>
-      <c r="X18" t="s">
+      <c r="X19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="15:24" ht="17">
-      <c r="U19" t="s">
+    <row r="20" spans="1:24" ht="17">
+      <c r="U20" t="s">
         <v>23</v>
       </c>
-      <c r="X19" t="s">
+      <c r="X20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="15:24" ht="17">
-      <c r="X20" t="s">
+    <row r="21" spans="1:24" ht="17">
+      <c r="X21" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="17">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" t="s">
+        <v>10</v>
+      </c>
+      <c r="R26" t="s">
+        <v>18</v>
+      </c>
+      <c r="U26" t="s">
+        <v>20</v>
+      </c>
+      <c r="X26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" ht="17">
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27" t="s">
+        <v>36</v>
+      </c>
+      <c r="R27" t="s">
+        <v>39</v>
+      </c>
+      <c r="U27" t="s">
+        <v>46</v>
+      </c>
+      <c r="X27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" ht="17">
+      <c r="I28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O28" t="s">
+        <v>35</v>
+      </c>
+      <c r="R28" t="s">
+        <v>40</v>
+      </c>
+      <c r="U28" t="s">
+        <v>47</v>
+      </c>
+      <c r="X28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="17">
+      <c r="O29" t="s">
+        <v>34</v>
+      </c>
+      <c r="R29" t="s">
+        <v>41</v>
+      </c>
+      <c r="U29" t="s">
+        <v>48</v>
+      </c>
+      <c r="X29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="17">
+      <c r="R30" t="s">
+        <v>42</v>
+      </c>
+      <c r="U30" t="s">
+        <v>49</v>
+      </c>
+      <c r="X30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="17">
+      <c r="U31" t="s">
+        <v>50</v>
+      </c>
+      <c r="X31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" ht="17">
+      <c r="X32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" ht="17">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" t="s">
+        <v>67</v>
+      </c>
+      <c r="O36" t="s">
+        <v>68</v>
+      </c>
+      <c r="R36" t="s">
+        <v>69</v>
+      </c>
+      <c r="U36" t="s">
+        <v>70</v>
+      </c>
+      <c r="X36" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="17">
+      <c r="D37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I37" t="s">
+        <v>103</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" t="s">
+        <v>43</v>
+      </c>
+      <c r="U37" t="s">
+        <v>51</v>
+      </c>
+      <c r="X37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" ht="17">
+      <c r="I38" t="s">
+        <v>102</v>
+      </c>
+      <c r="O38" t="s">
+        <v>38</v>
+      </c>
+      <c r="R38" t="s">
+        <v>44</v>
+      </c>
+      <c r="U38" t="s">
+        <v>52</v>
+      </c>
+      <c r="X38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="17">
+      <c r="O39" t="s">
+        <v>73</v>
+      </c>
+      <c r="R39" t="s">
+        <v>45</v>
+      </c>
+      <c r="U39" t="s">
+        <v>53</v>
+      </c>
+      <c r="X39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="17">
+      <c r="R40" t="s">
+        <v>74</v>
+      </c>
+      <c r="U40" t="s">
+        <v>54</v>
+      </c>
+      <c r="X40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" ht="17">
+      <c r="U41" t="s">
+        <v>75</v>
+      </c>
+      <c r="X41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="17">
+      <c r="X42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" ht="17">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" t="s">
+        <v>99</v>
+      </c>
+      <c r="O46" t="s">
+        <v>106</v>
+      </c>
+      <c r="R46" t="s">
+        <v>77</v>
+      </c>
+      <c r="U46" t="s">
+        <v>91</v>
+      </c>
+      <c r="X46" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" ht="17">
+      <c r="D47" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" t="s">
+        <v>104</v>
+      </c>
+      <c r="O47" t="s">
+        <v>83</v>
+      </c>
+      <c r="R47" t="s">
+        <v>78</v>
+      </c>
+      <c r="U47" t="s">
+        <v>86</v>
+      </c>
+      <c r="X47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" ht="17">
+      <c r="I48" t="s">
+        <v>105</v>
+      </c>
+      <c r="O48" t="s">
+        <v>84</v>
+      </c>
+      <c r="R48" t="s">
+        <v>79</v>
+      </c>
+      <c r="U48" t="s">
+        <v>87</v>
+      </c>
+      <c r="X48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="4:24" ht="17">
+      <c r="O49" t="s">
+        <v>85</v>
+      </c>
+      <c r="R49" t="s">
+        <v>80</v>
+      </c>
+      <c r="U49" t="s">
+        <v>88</v>
+      </c>
+      <c r="X49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="4:24" ht="17">
+      <c r="R50" t="s">
+        <v>81</v>
+      </c>
+      <c r="U50" t="s">
+        <v>89</v>
+      </c>
+      <c r="X50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="4:24" ht="17">
+      <c r="D51" s="9"/>
+      <c r="U51" t="s">
+        <v>90</v>
+      </c>
+      <c r="X51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="4:24" ht="17">
+      <c r="D52" s="3"/>
+      <c r="X52" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>